<commit_message>
text replace (RAIS, RAII)
title change
</commit_message>
<xml_diff>
--- a/RAII Framework.xlsx
+++ b/RAII Framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leah/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leah/Documents/RAII Framework/RAII-Framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DB28B7-5E46-5E4B-AEAA-03792FB79CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3EFC6-CCFA-8E48-AD11-0AC68672CF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="640" windowWidth="19800" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6140" yWindow="640" windowWidth="19800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Risk Assessment" sheetId="1" r:id="rId1"/>
@@ -209,6 +209,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Initial</t>
     </r>
@@ -217,6 +218,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> risk</t>
     </r>
@@ -236,6 +238,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Remaining</t>
     </r>
@@ -244,6 +247,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> risk</t>
     </r>
@@ -296,6 +300,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Initial</t>
     </r>
@@ -304,6 +309,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> risk</t>
     </r>
@@ -323,6 +329,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Remaining</t>
     </r>
@@ -331,6 +338,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> risk</t>
     </r>
@@ -419,9 +427,6 @@
   </si>
   <si>
     <t>Risk Assessment: Industry-Specific and Regulatory</t>
-  </si>
-  <si>
-    <t>RESPONSIBLE AI INVESTING and SAFETY (RAIS) FRAMEWORK</t>
   </si>
   <si>
     <t xml:space="preserve">Radical Ventures, 2023 </t>
@@ -617,6 +622,9 @@
   <si>
     <t>Describe vulnerabilities associated with the company's management team including track record, diversity in skillsets, as well as considerations for diversity, equity, and inclusion, and codifying  decision-making processes.</t>
   </si>
+  <si>
+    <t>RESPONSIBLE AI INVESTING (RAII) FRAMEWORK</t>
+  </si>
 </sst>
 </file>
 
@@ -633,74 +641,87 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF993300"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF008080"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF862303"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -712,6 +733,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1435,13 +1457,134 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1457,149 +1600,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1616,8 +1638,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF9900"/>
           <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1632,8 +1670,32 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1656,8 +1718,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF9900"/>
           <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1672,8 +1750,32 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1696,8 +1798,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF9900"/>
           <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1712,24 +1830,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1744,14 +1846,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
         </patternFill>
@@ -1760,80 +1854,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2093,8 +2115,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2128,12 +2150,12 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
-      <c r="A2" s="119" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
+      <c r="A2" s="135" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2148,10 +2170,10 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A3" s="119"/>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
+      <c r="A3" s="135"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2166,12 +2188,12 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A4" s="122" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
+      <c r="A4" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2256,7 +2278,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="15">
       <c r="A8" s="11"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2302,7 +2324,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="15">
       <c r="A10" s="11"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2367,7 +2389,7 @@
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="17">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="105" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="18"/>
@@ -2387,7 +2409,7 @@
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="19">
-      <c r="A14" s="129" t="s">
+      <c r="A14" s="106" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="20">
@@ -2429,7 +2451,7 @@
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="19">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="106" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="20">
@@ -2472,7 +2494,7 @@
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="19">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="106" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="20">
@@ -2515,7 +2537,7 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="19">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="107" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="20">
@@ -2558,7 +2580,7 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="19">
-      <c r="A18" s="129" t="s">
+      <c r="A18" s="106" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="20">
@@ -2601,7 +2623,7 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" ht="19">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="106" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="20">
@@ -2644,7 +2666,7 @@
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" ht="19">
-      <c r="A20" s="129" t="s">
+      <c r="A20" s="106" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="20">
@@ -2687,7 +2709,7 @@
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" ht="19">
-      <c r="A21" s="131"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="27"/>
       <c r="C21" s="28">
         <v>1</v>
@@ -2718,39 +2740,39 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" s="127" customFormat="1" ht="51">
-      <c r="A22" s="123"/>
-      <c r="B22" s="124" t="s">
+    <row r="22" spans="1:16" s="104" customFormat="1" ht="51">
+      <c r="A22" s="100"/>
+      <c r="B22" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="125" t="s">
+      <c r="D22" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="125" t="s">
+      <c r="E22" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="125" t="s">
+      <c r="F22" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="125" t="s">
+      <c r="G22" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="125" t="s">
+      <c r="H22" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="125" t="s">
+      <c r="I22" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="123"/>
-      <c r="K22" s="126"/>
-      <c r="L22" s="126"/>
-      <c r="M22" s="126"/>
-      <c r="N22" s="126"/>
-      <c r="O22" s="126"/>
-      <c r="P22" s="126"/>
+      <c r="J22" s="100"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="103"/>
+      <c r="M22" s="103"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="103"/>
     </row>
     <row r="23" spans="1:16" ht="16" thickBot="1">
       <c r="A23" s="29"/>
@@ -2797,9 +2819,9 @@
       <c r="B25" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="93"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2841,9 +2863,9 @@
       <c r="B27" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="91"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="93"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="131"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2863,9 +2885,9 @@
       <c r="B28" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="93"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="131"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2885,9 +2907,9 @@
       <c r="B29" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="94"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="96"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="134"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2900,7 +2922,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2919,17 +2941,17 @@
       <c r="P30" s="1"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="120"/>
-      <c r="B34" s="120"/>
+      <c r="A34" s="128"/>
+      <c r="B34" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:D3"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A2:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B11">
     <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThanOrEqual">
@@ -2959,7 +2981,7 @@
   </sheetPr>
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2973,22 +2995,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
     </row>
     <row r="2" spans="1:21" ht="45" customHeight="1">
       <c r="A2" s="43"/>
@@ -3007,10 +3029,10 @@
       <c r="F2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="98" t="s">
+      <c r="G2" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="99"/>
+      <c r="H2" s="140"/>
       <c r="I2" s="46" t="s">
         <v>36</v>
       </c>
@@ -3042,11 +3064,11 @@
         <f t="shared" ref="F3:F10" si="0">$D3*$E3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="134" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="134" t="s">
-        <v>87</v>
+      <c r="G3" s="111" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="111" t="s">
+        <v>86</v>
       </c>
       <c r="I3" s="53">
         <v>3</v>
@@ -3234,11 +3256,11 @@
     </row>
     <row r="9" spans="1:21" ht="64">
       <c r="A9" s="48"/>
-      <c r="B9" s="135" t="s">
+      <c r="B9" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="109" t="s">
         <v>111</v>
-      </c>
-      <c r="C9" s="132" t="s">
-        <v>112</v>
       </c>
       <c r="D9" s="51">
         <v>7</v>
@@ -3259,11 +3281,11 @@
     </row>
     <row r="10" spans="1:21" ht="96">
       <c r="A10" s="48"/>
-      <c r="B10" s="135" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="132" t="s">
-        <v>113</v>
+      <c r="B10" s="112" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>112</v>
       </c>
       <c r="D10" s="51">
         <v>3</v>
@@ -3285,7 +3307,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="13"/>
-    <row r="12" spans="1:21" ht="32">
+    <row r="12" spans="1:21" ht="31">
       <c r="A12" s="60"/>
       <c r="B12" s="61"/>
       <c r="C12" s="62" t="s">
@@ -3337,12 +3359,12 @@
       <c r="C16" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="93"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
+      <c r="G16" s="131"/>
     </row>
     <row r="17" spans="2:9" ht="16">
       <c r="B17" s="71" t="s">
@@ -3351,12 +3373,12 @@
       <c r="C17" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="D17" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="93"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="131"/>
     </row>
     <row r="18" spans="2:9" ht="16">
       <c r="B18" s="71" t="s">
@@ -3365,12 +3387,12 @@
       <c r="C18" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="93"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="131"/>
     </row>
     <row r="19" spans="2:9" ht="16">
       <c r="B19" s="71" t="s">
@@ -3379,12 +3401,12 @@
       <c r="C19" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="131"/>
     </row>
     <row r="20" spans="2:9" ht="16">
       <c r="B20" s="76" t="s">
@@ -3393,12 +3415,12 @@
       <c r="C20" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="96"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="134"/>
     </row>
     <row r="21" spans="2:9" ht="15">
       <c r="B21" s="78"/>
@@ -3440,8 +3462,8 @@
       <c r="B24" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="140" t="s">
-        <v>90</v>
+      <c r="C24" s="117" t="s">
+        <v>89</v>
       </c>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
@@ -3454,8 +3476,8 @@
       <c r="B25" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="140" t="s">
-        <v>91</v>
+      <c r="C25" s="117" t="s">
+        <v>90</v>
       </c>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
@@ -3468,8 +3490,8 @@
       <c r="B26" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="140" t="s">
-        <v>92</v>
+      <c r="C26" s="117" t="s">
+        <v>91</v>
       </c>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
@@ -3482,8 +3504,8 @@
       <c r="B27" s="83">
         <v>7</v>
       </c>
-      <c r="C27" s="141" t="s">
-        <v>93</v>
+      <c r="C27" s="118" t="s">
+        <v>92</v>
       </c>
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
@@ -3507,39 +3529,39 @@
       <formula>0</formula>
       <formula>10.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="between">
+      <formula>40.5</formula>
+      <formula>50.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="26" priority="7" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="between">
-      <formula>40.5</formula>
-      <formula>50.5</formula>
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K10 M11 K12">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>10.5</formula>
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="4" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>10.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="10" operator="between">
       <formula>40.5</formula>
@@ -3566,59 +3588,59 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="108" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="108" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" style="108" customWidth="1"/>
-    <col min="4" max="8" width="12.6640625" style="108"/>
-    <col min="9" max="9" width="31.1640625" style="108" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" style="108" customWidth="1"/>
-    <col min="11" max="16384" width="12.6640625" style="108"/>
+    <col min="1" max="1" width="3.6640625" style="91" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="91" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="91" customWidth="1"/>
+    <col min="4" max="8" width="12.6640625" style="91"/>
+    <col min="9" max="9" width="31.1640625" style="91" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="91" customWidth="1"/>
+    <col min="11" max="16384" width="12.6640625" style="91"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
     </row>
     <row r="2" spans="1:21" ht="48">
-      <c r="A2" s="109"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="44" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="138" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="138" t="s">
-        <v>84</v>
+      <c r="D2" s="115" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="115" t="s">
+        <v>83</v>
       </c>
       <c r="F2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="110"/>
-      <c r="I2" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="139" t="s">
-        <v>85</v>
+      <c r="H2" s="149"/>
+      <c r="I2" s="116" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="116" t="s">
+        <v>84</v>
       </c>
       <c r="K2" s="46" t="s">
         <v>2</v>
@@ -3629,11 +3651,11 @@
     </row>
     <row r="3" spans="1:21" ht="112">
       <c r="A3" s="48"/>
-      <c r="B3" s="133" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="132" t="s">
-        <v>86</v>
+      <c r="B3" s="110" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="109" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="51">
         <v>3</v>
@@ -3645,11 +3667,11 @@
         <f t="shared" ref="F3:F14" si="0">$D3*$E3</f>
         <v>15</v>
       </c>
-      <c r="G3" s="134" t="s">
+      <c r="G3" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="111" t="s">
         <v>88</v>
-      </c>
-      <c r="H3" s="134" t="s">
-        <v>89</v>
       </c>
       <c r="I3" s="53">
         <v>5</v>
@@ -3667,11 +3689,11 @@
     </row>
     <row r="4" spans="1:21" ht="192">
       <c r="A4" s="48"/>
-      <c r="B4" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="136" t="s">
-        <v>83</v>
+      <c r="B4" s="114" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>82</v>
       </c>
       <c r="D4" s="51">
         <v>3</v>
@@ -3900,14 +3922,14 @@
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:21" ht="13"/>
-    <row r="16" spans="1:21" ht="32">
+    <row r="16" spans="1:21" ht="31">
       <c r="A16" s="90"/>
-      <c r="B16" s="111"/>
+      <c r="B16" s="93"/>
       <c r="C16" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
       <c r="F16" s="64">
         <f>AVERAGEIF(F3:F14,"&gt;0")</f>
         <v>15</v>
@@ -3916,8 +3938,8 @@
         <v>66</v>
       </c>
       <c r="H16" s="65"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="112"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
       <c r="K16" s="67">
         <f>AVERAGEIF(K3:K14,"&gt;0")</f>
         <v>15</v>
@@ -3939,11 +3961,11 @@
       <c r="B19" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="114"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="96"/>
     </row>
     <row r="20" spans="2:9" ht="16">
       <c r="B20" s="71" t="s">
@@ -3952,12 +3974,12 @@
       <c r="C20" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="145"/>
     </row>
     <row r="21" spans="2:9" ht="31" customHeight="1">
       <c r="B21" s="71" t="s">
@@ -3966,12 +3988,12 @@
       <c r="C21" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="116"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="144"/>
+      <c r="G21" s="145"/>
     </row>
     <row r="22" spans="2:9" ht="16">
       <c r="B22" s="71" t="s">
@@ -3980,12 +4002,12 @@
       <c r="C22" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="116"/>
+      <c r="E22" s="144"/>
+      <c r="F22" s="144"/>
+      <c r="G22" s="145"/>
     </row>
     <row r="23" spans="2:9" ht="16">
       <c r="B23" s="71" t="s">
@@ -3994,12 +4016,12 @@
       <c r="C23" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="103" t="s">
+      <c r="D23" s="136" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="115"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="116"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
     </row>
     <row r="24" spans="2:9" ht="16">
       <c r="B24" s="76" t="s">
@@ -4008,16 +4030,16 @@
       <c r="C24" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="137" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="117"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="147"/>
     </row>
     <row r="25" spans="2:9" ht="15">
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="90"/>
       <c r="E25" s="90"/>
       <c r="F25" s="90"/>
@@ -4055,8 +4077,8 @@
       <c r="B28" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="140" t="s">
-        <v>94</v>
+      <c r="C28" s="117" t="s">
+        <v>93</v>
       </c>
       <c r="D28" s="90"/>
       <c r="E28" s="90"/>
@@ -4069,8 +4091,8 @@
       <c r="B29" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="140" t="s">
-        <v>95</v>
+      <c r="C29" s="117" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="90"/>
       <c r="E29" s="90"/>
@@ -4083,8 +4105,8 @@
       <c r="B30" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="140" t="s">
-        <v>96</v>
+      <c r="C30" s="117" t="s">
+        <v>95</v>
       </c>
       <c r="D30" s="90"/>
       <c r="E30" s="90"/>
@@ -4097,8 +4119,8 @@
       <c r="B31" s="83">
         <v>7</v>
       </c>
-      <c r="C31" s="141" t="s">
-        <v>97</v>
+      <c r="C31" s="118" t="s">
+        <v>96</v>
       </c>
       <c r="D31" s="90"/>
       <c r="E31" s="90"/>
@@ -4122,39 +4144,39 @@
       <formula>0</formula>
       <formula>10.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="between">
+      <formula>40.5</formula>
+      <formula>50.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="7" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="between">
-      <formula>40.5</formula>
-      <formula>50.5</formula>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K14 M15 K16">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>10.5</formula>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="13" priority="4" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>10.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="10" operator="between">
       <formula>40.5</formula>
@@ -4190,23 +4212,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14" thickBot="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="150" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
+      <c r="L1" s="151"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
     </row>
     <row r="2" spans="1:21" ht="32">
       <c r="A2" s="43"/>
@@ -4225,31 +4247,31 @@
       <c r="F2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="98" t="s">
+      <c r="G2" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="I2" s="149" t="s">
+      <c r="H2" s="130"/>
+      <c r="I2" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="149" t="s">
+      <c r="J2" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="149" t="s">
+      <c r="K2" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="150" t="s">
+      <c r="L2" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="145"/>
+      <c r="M2" s="122"/>
     </row>
     <row r="3" spans="1:21" ht="128">
       <c r="A3" s="48"/>
       <c r="B3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="132" t="s">
-        <v>98</v>
+      <c r="C3" s="109" t="s">
+        <v>97</v>
       </c>
       <c r="D3" s="51">
         <v>1</v>
@@ -4261,19 +4283,19 @@
         <f t="shared" ref="F3:F14" si="0">$D3*$E3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="134" t="s">
+      <c r="G3" s="111" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="134" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" s="147">
+      <c r="I3" s="123">
         <v>5</v>
       </c>
-      <c r="J3" s="147">
+      <c r="J3" s="123">
         <v>3</v>
       </c>
-      <c r="K3" s="148">
+      <c r="K3" s="124">
         <f t="shared" ref="K3:K14" si="1">$I3*$J3</f>
         <v>15</v>
       </c>
@@ -4283,11 +4305,11 @@
     </row>
     <row r="4" spans="1:21" ht="112">
       <c r="A4" s="48"/>
-      <c r="B4" s="143" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="142" t="s">
-        <v>104</v>
+      <c r="B4" s="120" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="119" t="s">
+        <v>103</v>
       </c>
       <c r="D4" s="51">
         <v>3</v>
@@ -4317,11 +4339,11 @@
     </row>
     <row r="5" spans="1:21" ht="112">
       <c r="A5" s="48"/>
-      <c r="B5" s="135" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="136" t="s">
-        <v>105</v>
+      <c r="B5" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="113" t="s">
+        <v>104</v>
       </c>
       <c r="D5" s="51">
         <v>3</v>
@@ -4351,11 +4373,11 @@
     </row>
     <row r="6" spans="1:21" ht="96">
       <c r="A6" s="48"/>
-      <c r="B6" s="135" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="136" t="s">
-        <v>106</v>
+      <c r="B6" s="112" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="113" t="s">
+        <v>105</v>
       </c>
       <c r="D6" s="51">
         <v>3</v>
@@ -4385,11 +4407,11 @@
     </row>
     <row r="7" spans="1:21" ht="64">
       <c r="A7" s="48"/>
-      <c r="B7" s="144" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="136" t="s">
+      <c r="B7" s="121" t="s">
         <v>107</v>
+      </c>
+      <c r="C7" s="113" t="s">
+        <v>106</v>
       </c>
       <c r="D7" s="51">
         <v>3</v>
@@ -4419,11 +4441,11 @@
     </row>
     <row r="8" spans="1:21" ht="80">
       <c r="A8" s="48"/>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="136" t="s">
-        <v>109</v>
+      <c r="C8" s="113" t="s">
+        <v>108</v>
       </c>
       <c r="D8" s="51">
         <v>3</v>
@@ -4453,7 +4475,7 @@
     </row>
     <row r="9" spans="1:21" ht="15">
       <c r="A9" s="48"/>
-      <c r="B9" s="135"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="87"/>
       <c r="D9" s="51"/>
       <c r="E9" s="51"/>
@@ -4572,7 +4594,7 @@
       <c r="L14" s="55"/>
     </row>
     <row r="15" spans="1:21" ht="13"/>
-    <row r="16" spans="1:21" ht="48">
+    <row r="16" spans="1:21" ht="46">
       <c r="A16" s="60"/>
       <c r="B16" s="61"/>
       <c r="C16" s="89" t="s">
@@ -4584,7 +4606,7 @@
         <f>AVERAGEIF(F3:F14,"&gt;0")</f>
         <v>14.666666666666666</v>
       </c>
-      <c r="G16" s="151" t="s">
+      <c r="G16" s="127" t="s">
         <v>75</v>
       </c>
       <c r="H16" s="66"/>
@@ -4624,12 +4646,12 @@
       <c r="C20" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="93"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="131"/>
     </row>
     <row r="21" spans="2:10" ht="16">
       <c r="B21" s="71" t="s">
@@ -4638,12 +4660,12 @@
       <c r="C21" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="92"/>
-      <c r="F21" s="92"/>
-      <c r="G21" s="93"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="131"/>
     </row>
     <row r="22" spans="2:10" ht="16">
       <c r="B22" s="71" t="s">
@@ -4652,12 +4674,12 @@
       <c r="C22" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="93"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="131"/>
     </row>
     <row r="23" spans="2:10" ht="16">
       <c r="B23" s="71" t="s">
@@ -4666,12 +4688,12 @@
       <c r="C23" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="103" t="s">
+      <c r="D23" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="93"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="131"/>
     </row>
     <row r="24" spans="2:10" ht="16">
       <c r="B24" s="76" t="s">
@@ -4680,12 +4702,12 @@
       <c r="C24" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="96"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="134"/>
     </row>
     <row r="25" spans="2:10" ht="15">
       <c r="B25" s="78"/>
@@ -4730,8 +4752,8 @@
       <c r="B28" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="140" t="s">
-        <v>90</v>
+      <c r="C28" s="117" t="s">
+        <v>89</v>
       </c>
       <c r="D28" s="90"/>
       <c r="E28" s="60"/>
@@ -4745,8 +4767,8 @@
       <c r="B29" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="140" t="s">
-        <v>91</v>
+      <c r="C29" s="117" t="s">
+        <v>90</v>
       </c>
       <c r="D29" s="90"/>
       <c r="E29" s="60"/>
@@ -4760,8 +4782,8 @@
       <c r="B30" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="140" t="s">
-        <v>92</v>
+      <c r="C30" s="117" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="90"/>
       <c r="E30" s="60"/>
@@ -4775,8 +4797,8 @@
       <c r="B31" s="83">
         <v>7</v>
       </c>
-      <c r="C31" s="141" t="s">
-        <v>93</v>
+      <c r="C31" s="118" t="s">
+        <v>92</v>
       </c>
       <c r="D31" s="90"/>
       <c r="E31" s="60"/>
@@ -4801,39 +4823,39 @@
       <formula>0</formula>
       <formula>10.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+      <formula>40.5</formula>
+      <formula>50.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="between">
-      <formula>40.5</formula>
-      <formula>50.5</formula>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K14 M15 K16">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>10.5</formula>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+      <formula>20.5</formula>
+      <formula>30.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>10.5</formula>
       <formula>20.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
-      <formula>20.5</formula>
-      <formula>30.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="between">
       <formula>30.5</formula>
       <formula>40.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>10.5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="10" operator="between">
       <formula>40.5</formula>

</xml_diff>